<commit_message>
feat: Add data integration to instructor profile
</commit_message>
<xml_diff>
--- a/02.Design Document/Project Management.xlsx
+++ b/02.Design Document/Project Management.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/Level-Up/02.Design Document/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/level-up-docs/02.Design Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB636B54-D2EF-B74F-886B-947EBA8CB372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C14E024-B721-C248-921B-E9DD590AA0A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4820" yWindow="-20940" windowWidth="33500" windowHeight="20460" activeTab="2" xr2:uid="{7BA0B221-245C-954E-96F6-3D960DADD312}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{7BA0B221-245C-954E-96F6-3D960DADD312}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -37,14 +37,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1732,6 +1724,12 @@
     <xf numFmtId="164" fontId="22" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="14" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="15" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1854,12 +1852,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="15" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -10378,9 +10370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAFE950-5B3C-524E-9704-0609BF069824}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10473,22 +10463,22 @@
       <c r="N18" s="13"/>
     </row>
     <row r="19" spans="1:14" ht="92" x14ac:dyDescent="0.2">
-      <c r="A19" s="134" t="s">
+      <c r="A19" s="140" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="135"/>
-      <c r="C19" s="135"/>
-      <c r="D19" s="135"/>
-      <c r="E19" s="135"/>
-      <c r="F19" s="135"/>
-      <c r="G19" s="135"/>
-      <c r="H19" s="135"/>
-      <c r="I19" s="135"/>
-      <c r="J19" s="135"/>
-      <c r="K19" s="135"/>
-      <c r="L19" s="135"/>
-      <c r="M19" s="135"/>
-      <c r="N19" s="136"/>
+      <c r="B19" s="141"/>
+      <c r="C19" s="141"/>
+      <c r="D19" s="141"/>
+      <c r="E19" s="141"/>
+      <c r="F19" s="141"/>
+      <c r="G19" s="141"/>
+      <c r="H19" s="141"/>
+      <c r="I19" s="141"/>
+      <c r="J19" s="141"/>
+      <c r="K19" s="141"/>
+      <c r="L19" s="141"/>
+      <c r="M19" s="141"/>
+      <c r="N19" s="142"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
@@ -10507,22 +10497,22 @@
       <c r="N21" s="13"/>
     </row>
     <row r="22" spans="1:14" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="131" t="s">
+      <c r="A22" s="137" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="132"/>
-      <c r="C22" s="132"/>
-      <c r="D22" s="132"/>
-      <c r="E22" s="132"/>
-      <c r="F22" s="132"/>
-      <c r="G22" s="132"/>
-      <c r="H22" s="132"/>
-      <c r="I22" s="132"/>
-      <c r="J22" s="132"/>
-      <c r="K22" s="132"/>
-      <c r="L22" s="132"/>
-      <c r="M22" s="132"/>
-      <c r="N22" s="133"/>
+      <c r="B22" s="138"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="138"/>
+      <c r="H22" s="138"/>
+      <c r="I22" s="138"/>
+      <c r="J22" s="138"/>
+      <c r="K22" s="138"/>
+      <c r="L22" s="138"/>
+      <c r="M22" s="138"/>
+      <c r="N22" s="139"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
@@ -10605,10 +10595,10 @@
     </row>
     <row r="42" spans="1:14" ht="24" x14ac:dyDescent="0.3">
       <c r="A42" s="12"/>
-      <c r="B42" s="129" t="s">
+      <c r="B42" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="129"/>
+      <c r="C42" s="135"/>
       <c r="D42" s="18">
         <v>1</v>
       </c>
@@ -10669,10 +10659,10 @@
     </row>
     <row r="48" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
-      <c r="K48" s="130" t="s">
+      <c r="K48" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="L48" s="130"/>
+      <c r="L48" s="136"/>
       <c r="M48" s="17">
         <v>44740</v>
       </c>
@@ -10680,10 +10670,10 @@
     </row>
     <row r="49" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
-      <c r="K49" s="130" t="s">
+      <c r="K49" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="L49" s="130"/>
+      <c r="L49" s="136"/>
       <c r="M49" s="17"/>
       <c r="N49" s="13"/>
     </row>
@@ -10737,56 +10727,56 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="143" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="141" t="str">
+      <c r="B2" s="144"/>
+      <c r="C2" s="147" t="str">
         <f>Cover!E40</f>
         <v xml:space="preserve">Level Up </v>
       </c>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="142"/>
-      <c r="L2" s="142"/>
-      <c r="M2" s="142"/>
-      <c r="N2" s="142"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
+      <c r="L2" s="148"/>
+      <c r="M2" s="148"/>
+      <c r="N2" s="148"/>
       <c r="O2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="145">
+      <c r="P2" s="151">
         <v>44740</v>
       </c>
-      <c r="Q2" s="146"/>
+      <c r="Q2" s="152"/>
     </row>
     <row r="3" spans="1:17" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="139"/>
-      <c r="B3" s="140"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="144"/>
+      <c r="A3" s="145"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="150"/>
+      <c r="K3" s="150"/>
+      <c r="L3" s="150"/>
+      <c r="M3" s="150"/>
+      <c r="N3" s="150"/>
       <c r="O3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="147">
+      <c r="P3" s="153">
         <f ca="1">NOW()</f>
-        <v>44766.857009259256</v>
-      </c>
-      <c r="Q3" s="148"/>
+        <v>44769.489709606481</v>
+      </c>
+      <c r="Q3" s="154"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
@@ -11755,8 +11745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F39F5A-DF39-F541-B8C2-02BEDD153576}">
   <dimension ref="A1:O128"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A96" zoomScale="140" zoomScaleNormal="140" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="I72" sqref="F72:I111"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11775,47 +11765,47 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="141" t="str">
+      <c r="B2" s="144"/>
+      <c r="C2" s="147" t="str">
         <f>Cover!E40</f>
         <v xml:space="preserve">Level Up </v>
       </c>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="142"/>
-      <c r="L2" s="142"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
+      <c r="L2" s="148"/>
       <c r="M2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="145"/>
-      <c r="O2" s="146"/>
+      <c r="N2" s="151"/>
+      <c r="O2" s="152"/>
     </row>
     <row r="3" spans="1:15" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="139"/>
-      <c r="B3" s="140"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
+      <c r="A3" s="145"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="150"/>
+      <c r="K3" s="150"/>
+      <c r="L3" s="150"/>
       <c r="M3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="147"/>
-      <c r="O3" s="148"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="154"/>
     </row>
     <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -11904,7 +11894,7 @@
         <v>44747</v>
       </c>
       <c r="G7" s="58">
-        <f t="shared" ref="G7:G64" si="0">F7-E7</f>
+        <f t="shared" ref="G7:G15" si="0">F7-E7</f>
         <v>2</v>
       </c>
       <c r="H7" s="59"/>
@@ -11990,7 +11980,7 @@
     <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
       <c r="B10" s="109">
-        <f t="shared" ref="B10:B60" si="4">ROW()-8</f>
+        <f t="shared" ref="B10:B15" si="4">ROW()-8</f>
         <v>2</v>
       </c>
       <c r="C10" s="58" t="s">
@@ -12206,7 +12196,7 @@
     <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="56"/>
       <c r="B16" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" ref="B16:B60" si="7">ROW()-8</f>
         <v>8</v>
       </c>
       <c r="C16" s="58" t="s">
@@ -12222,7 +12212,7 @@
         <v>44748</v>
       </c>
       <c r="G16" s="58">
-        <f>F16-E16</f>
+        <f t="shared" ref="G16:G47" si="8">F16-E16</f>
         <v>1</v>
       </c>
       <c r="H16" s="59">
@@ -12232,7 +12222,7 @@
         <v>44748</v>
       </c>
       <c r="J16" s="60">
-        <f>I16-H16</f>
+        <f t="shared" ref="J16:J47" si="9">I16-H16</f>
         <v>1</v>
       </c>
       <c r="K16" s="61">
@@ -12242,7 +12232,7 @@
     <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="56"/>
       <c r="B17" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="C17" s="58" t="s">
@@ -12258,7 +12248,7 @@
         <v>44748</v>
       </c>
       <c r="G17" s="58">
-        <f>F17-E17</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H17" s="59">
@@ -12268,7 +12258,7 @@
         <v>44748</v>
       </c>
       <c r="J17" s="60">
-        <f>I17-H17</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K17" s="61">
@@ -12278,7 +12268,7 @@
     <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="56"/>
       <c r="B18" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="C18" s="58" t="s">
@@ -12294,7 +12284,7 @@
         <v>44749</v>
       </c>
       <c r="G18" s="58">
-        <f>F18-E18</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="H18" s="59">
@@ -12304,7 +12294,7 @@
         <v>44749</v>
       </c>
       <c r="J18" s="60">
-        <f>I18-H18</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K18" s="61">
@@ -12314,7 +12304,7 @@
     <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="56"/>
       <c r="B19" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="C19" s="58" t="s">
@@ -12330,7 +12320,7 @@
         <v>44749</v>
       </c>
       <c r="G19" s="58">
-        <f>F19-E19</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="H19" s="59">
@@ -12340,7 +12330,7 @@
         <v>44749</v>
       </c>
       <c r="J19" s="60">
-        <f>I19-H19</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K19" s="61">
@@ -12350,7 +12340,7 @@
     <row r="20" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="56"/>
       <c r="B20" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="C20" s="58" t="s">
@@ -12366,7 +12356,7 @@
         <v>44749</v>
       </c>
       <c r="G20" s="58">
-        <f>F20-E20</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H20" s="59">
@@ -12376,7 +12366,7 @@
         <v>44749</v>
       </c>
       <c r="J20" s="60">
-        <f>I20-H20</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K20" s="61">
@@ -12386,7 +12376,7 @@
     <row r="21" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="56"/>
       <c r="B21" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="C21" s="58" t="s">
@@ -12402,7 +12392,7 @@
         <v>44750</v>
       </c>
       <c r="G21" s="58">
-        <f>F21-E21</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H21" s="59">
@@ -12412,7 +12402,7 @@
         <v>44750</v>
       </c>
       <c r="J21" s="60">
-        <f>I21-H21</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K21" s="61">
@@ -12422,7 +12412,7 @@
     <row r="22" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="56"/>
       <c r="B22" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="C22" s="58" t="s">
@@ -12438,7 +12428,7 @@
         <v>44750</v>
       </c>
       <c r="G22" s="58">
-        <f>F22-E22</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="H22" s="59">
@@ -12448,7 +12438,7 @@
         <v>44750</v>
       </c>
       <c r="J22" s="60">
-        <f>I22-H22</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K22" s="61">
@@ -12458,7 +12448,7 @@
     <row r="23" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="56"/>
       <c r="B23" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="C23" s="58" t="s">
@@ -12474,7 +12464,7 @@
         <v>44751</v>
       </c>
       <c r="G23" s="58">
-        <f>F23-E23</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H23" s="59">
@@ -12484,7 +12474,7 @@
         <v>44750</v>
       </c>
       <c r="J23" s="60">
-        <f>I23-H23</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K23" s="61">
@@ -12494,7 +12484,7 @@
     <row r="24" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="56"/>
       <c r="B24" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="C24" s="58" t="s">
@@ -12510,7 +12500,7 @@
         <v>44750</v>
       </c>
       <c r="G24" s="58">
-        <f>F24-E24</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="H24" s="59">
@@ -12520,7 +12510,7 @@
         <v>44749</v>
       </c>
       <c r="J24" s="60">
-        <f>I24-H24</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K24" s="61">
@@ -12530,7 +12520,7 @@
     <row r="25" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="56"/>
       <c r="B25" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
       <c r="C25" s="58" t="s">
@@ -12546,7 +12536,7 @@
         <v>44751</v>
       </c>
       <c r="G25" s="58">
-        <f>F25-E25</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H25" s="59">
@@ -12556,7 +12546,7 @@
         <v>44750</v>
       </c>
       <c r="J25" s="60">
-        <f>I25-H25</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K25" s="61">
@@ -12566,7 +12556,7 @@
     <row r="26" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="56"/>
       <c r="B26" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="C26" s="58" t="s">
@@ -12582,7 +12572,7 @@
         <v>44750</v>
       </c>
       <c r="G26" s="58">
-        <f>F26-E26</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H26" s="59">
@@ -12592,7 +12582,7 @@
         <v>44750</v>
       </c>
       <c r="J26" s="60">
-        <f>I26-H26</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K26" s="61">
@@ -12602,7 +12592,7 @@
     <row r="27" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="56"/>
       <c r="B27" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
       <c r="C27" s="58" t="s">
@@ -12618,7 +12608,7 @@
         <v>44751</v>
       </c>
       <c r="G27" s="58">
-        <f>F27-E27</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H27" s="59">
@@ -12628,7 +12618,7 @@
         <v>44751</v>
       </c>
       <c r="J27" s="60">
-        <f>I27-H27</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K27" s="61">
@@ -12638,7 +12628,7 @@
     <row r="28" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="56"/>
       <c r="B28" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="C28" s="58" t="s">
@@ -12654,7 +12644,7 @@
         <v>44752</v>
       </c>
       <c r="G28" s="58">
-        <f>F28-E28</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H28" s="59">
@@ -12664,7 +12654,7 @@
         <v>44751</v>
       </c>
       <c r="J28" s="60">
-        <f>I28-H28</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K28" s="61">
@@ -12674,7 +12664,7 @@
     <row r="29" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="56"/>
       <c r="B29" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
       <c r="C29" s="58" t="s">
@@ -12690,7 +12680,7 @@
         <v>44752</v>
       </c>
       <c r="G29" s="58">
-        <f>F29-E29</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H29" s="59">
@@ -12700,7 +12690,7 @@
         <v>44752</v>
       </c>
       <c r="J29" s="60">
-        <f>I29-H29</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K29" s="61">
@@ -12710,7 +12700,7 @@
     <row r="30" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="56"/>
       <c r="B30" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="C30" s="58" t="s">
@@ -12726,7 +12716,7 @@
         <v>44752</v>
       </c>
       <c r="G30" s="58">
-        <f>F30-E30</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H30" s="59">
@@ -12736,7 +12726,7 @@
         <v>44749</v>
       </c>
       <c r="J30" s="60">
-        <f>I30-H30</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K30" s="61">
@@ -12746,7 +12736,7 @@
     <row r="31" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="56"/>
       <c r="B31" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
       <c r="C31" s="58" t="s">
@@ -12762,7 +12752,7 @@
         <v>44752</v>
       </c>
       <c r="G31" s="58">
-        <f>F31-E31</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H31" s="59">
@@ -12772,7 +12762,7 @@
         <v>44748</v>
       </c>
       <c r="J31" s="60">
-        <f>I31-H31</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="K31" s="61">
@@ -12782,7 +12772,7 @@
     <row r="32" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="56"/>
       <c r="B32" s="109">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="C32" s="58" t="s">
@@ -12798,7 +12788,7 @@
         <v>44752</v>
       </c>
       <c r="G32" s="58">
-        <f>F32-E32</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H32" s="59">
@@ -12808,7 +12798,7 @@
         <v>44752</v>
       </c>
       <c r="J32" s="60">
-        <f>I32-H32</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K32" s="61">
@@ -12818,7 +12808,7 @@
     <row r="33" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="56"/>
       <c r="B33" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
       <c r="C33" s="58" t="s">
@@ -12834,7 +12824,7 @@
         <v>44750</v>
       </c>
       <c r="G33" s="58">
-        <f>F33-E33</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H33" s="59">
@@ -12844,7 +12834,7 @@
         <v>44750</v>
       </c>
       <c r="J33" s="60">
-        <f>I33-H33</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K33" s="61">
@@ -12854,7 +12844,7 @@
     <row r="34" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="56"/>
       <c r="B34" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="C34" s="58" t="s">
@@ -12870,7 +12860,7 @@
         <v>44749</v>
       </c>
       <c r="G34" s="58">
-        <f>F34-E34</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H34" s="59">
@@ -12880,7 +12870,7 @@
         <v>44748</v>
       </c>
       <c r="J34" s="60">
-        <f>I34-H34</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K34" s="61">
@@ -12890,7 +12880,7 @@
     <row r="35" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="56"/>
       <c r="B35" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="C35" s="58" t="s">
@@ -12906,7 +12896,7 @@
         <v>44750</v>
       </c>
       <c r="G35" s="58">
-        <f>F35-E35</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H35" s="59">
@@ -12916,7 +12906,7 @@
         <v>44750</v>
       </c>
       <c r="J35" s="60">
-        <f>I35-H35</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K35" s="61">
@@ -12926,7 +12916,7 @@
     <row r="36" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="56"/>
       <c r="B36" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="C36" s="58" t="s">
@@ -12942,7 +12932,7 @@
         <v>44751</v>
       </c>
       <c r="G36" s="58">
-        <f>F36-E36</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H36" s="59">
@@ -12952,7 +12942,7 @@
         <v>44751</v>
       </c>
       <c r="J36" s="60">
-        <f>I36-H36</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K36" s="61">
@@ -12962,7 +12952,7 @@
     <row r="37" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="56"/>
       <c r="B37" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
       <c r="C37" s="58" t="s">
@@ -12978,7 +12968,7 @@
         <v>44751</v>
       </c>
       <c r="G37" s="58">
-        <f>F37-E37</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H37" s="59">
@@ -12988,7 +12978,7 @@
         <v>44751</v>
       </c>
       <c r="J37" s="60">
-        <f>I37-H37</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="K37" s="61">
@@ -12998,7 +12988,7 @@
     <row r="38" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="56"/>
       <c r="B38" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="C38" s="58" t="s">
@@ -13014,7 +13004,7 @@
         <v>44752</v>
       </c>
       <c r="G38" s="58">
-        <f>F38-E38</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H38" s="59">
@@ -13024,7 +13014,7 @@
         <v>44752</v>
       </c>
       <c r="J38" s="60">
-        <f>I38-H38</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K38" s="61">
@@ -13034,7 +13024,7 @@
     <row r="39" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="56"/>
       <c r="B39" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
       <c r="C39" s="58" t="s">
@@ -13050,7 +13040,7 @@
         <v>44752</v>
       </c>
       <c r="G39" s="58">
-        <f>F39-E39</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H39" s="59">
@@ -13060,7 +13050,7 @@
         <v>44752</v>
       </c>
       <c r="J39" s="60">
-        <f>I39-H39</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K39" s="61">
@@ -13070,7 +13060,7 @@
     <row r="40" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="56"/>
       <c r="B40" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
       <c r="C40" s="58" t="s">
@@ -13086,7 +13076,7 @@
         <v>44752</v>
       </c>
       <c r="G40" s="58">
-        <f>F40-E40</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H40" s="59">
@@ -13096,7 +13086,7 @@
         <v>44752</v>
       </c>
       <c r="J40" s="60">
-        <f>I40-H40</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K40" s="61">
@@ -13106,7 +13096,7 @@
     <row r="41" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="56"/>
       <c r="B41" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
       <c r="C41" s="58" t="s">
@@ -13122,7 +13112,7 @@
         <v>44753</v>
       </c>
       <c r="G41" s="58">
-        <f>F41-E41</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H41" s="59">
@@ -13132,7 +13122,7 @@
         <v>44753</v>
       </c>
       <c r="J41" s="60">
-        <f>I41-H41</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K41" s="61">
@@ -13142,7 +13132,7 @@
     <row r="42" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="56"/>
       <c r="B42" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
       <c r="C42" s="58" t="s">
@@ -13158,7 +13148,7 @@
         <v>44753</v>
       </c>
       <c r="G42" s="58">
-        <f>F42-E42</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H42" s="59">
@@ -13168,7 +13158,7 @@
         <v>44753</v>
       </c>
       <c r="J42" s="60">
-        <f>I42-H42</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K42" s="61">
@@ -13178,7 +13168,7 @@
     <row r="43" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="56"/>
       <c r="B43" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="C43" s="58" t="s">
@@ -13194,7 +13184,7 @@
         <v>44753</v>
       </c>
       <c r="G43" s="58">
-        <f>F43-E43</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H43" s="59">
@@ -13204,7 +13194,7 @@
         <v>44753</v>
       </c>
       <c r="J43" s="60">
-        <f>I43-H43</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K43" s="61">
@@ -13214,7 +13204,7 @@
     <row r="44" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="56"/>
       <c r="B44" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="C44" s="58" t="s">
@@ -13230,7 +13220,7 @@
         <v>44754</v>
       </c>
       <c r="G44" s="58">
-        <f>F44-E44</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H44" s="59">
@@ -13240,7 +13230,7 @@
         <v>44754</v>
       </c>
       <c r="J44" s="60">
-        <f>I44-H44</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K44" s="61">
@@ -13250,7 +13240,7 @@
     <row r="45" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="56"/>
       <c r="B45" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
       <c r="C45" s="58" t="s">
@@ -13266,7 +13256,7 @@
         <v>44754</v>
       </c>
       <c r="G45" s="58">
-        <f>F45-E45</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H45" s="59">
@@ -13276,7 +13266,7 @@
         <v>44754</v>
       </c>
       <c r="J45" s="60">
-        <f>I45-H45</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K45" s="61">
@@ -13286,7 +13276,7 @@
     <row r="46" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="56"/>
       <c r="B46" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>38</v>
       </c>
       <c r="C46" s="58" t="s">
@@ -13302,7 +13292,7 @@
         <v>44751</v>
       </c>
       <c r="G46" s="58">
-        <f>F46-E46</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H46" s="59">
@@ -13312,7 +13302,7 @@
         <v>44751</v>
       </c>
       <c r="J46" s="60">
-        <f>I46-H46</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K46" s="61">
@@ -13322,7 +13312,7 @@
     <row r="47" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="56"/>
       <c r="B47" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>39</v>
       </c>
       <c r="C47" s="58" t="s">
@@ -13338,7 +13328,7 @@
         <v>44752</v>
       </c>
       <c r="G47" s="58">
-        <f>F47-E47</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H47" s="59">
@@ -13348,7 +13338,7 @@
         <v>44751</v>
       </c>
       <c r="J47" s="60">
-        <f>I47-H47</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="K47" s="61">
@@ -13361,7 +13351,7 @@
     <row r="48" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="56"/>
       <c r="B48" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="C48" s="58" t="s">
@@ -13377,7 +13367,7 @@
         <v>44752</v>
       </c>
       <c r="G48" s="58">
-        <f>F48-E48</f>
+        <f t="shared" ref="G48:G79" si="10">F48-E48</f>
         <v>1</v>
       </c>
       <c r="H48" s="59">
@@ -13387,7 +13377,7 @@
         <v>44752</v>
       </c>
       <c r="J48" s="60">
-        <f>I48-H48</f>
+        <f t="shared" ref="J48:J79" si="11">I48-H48</f>
         <v>1</v>
       </c>
       <c r="K48" s="61">
@@ -13397,7 +13387,7 @@
     <row r="49" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="56"/>
       <c r="B49" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>41</v>
       </c>
       <c r="C49" s="58" t="s">
@@ -13413,7 +13403,7 @@
         <v>44752</v>
       </c>
       <c r="G49" s="58">
-        <f>F49-E49</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H49" s="59">
@@ -13423,7 +13413,7 @@
         <v>44752</v>
       </c>
       <c r="J49" s="60">
-        <f>I49-H49</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K49" s="61">
@@ -13433,7 +13423,7 @@
     <row r="50" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="56"/>
       <c r="B50" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
       <c r="C50" s="58" t="s">
@@ -13449,7 +13439,7 @@
         <v>44754</v>
       </c>
       <c r="G50" s="58">
-        <f>F50-E50</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H50" s="59">
@@ -13459,7 +13449,7 @@
         <v>44754</v>
       </c>
       <c r="J50" s="60">
-        <f>I50-H50</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K50" s="61">
@@ -13469,7 +13459,7 @@
     <row r="51" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="56"/>
       <c r="B51" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
       <c r="C51" s="58" t="s">
@@ -13485,7 +13475,7 @@
         <v>44754</v>
       </c>
       <c r="G51" s="58">
-        <f>F51-E51</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H51" s="59">
@@ -13495,7 +13485,7 @@
         <v>44754</v>
       </c>
       <c r="J51" s="60">
-        <f>I51-H51</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K51" s="61">
@@ -13505,7 +13495,7 @@
     <row r="52" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="56"/>
       <c r="B52" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
       <c r="C52" s="58" t="s">
@@ -13521,7 +13511,7 @@
         <v>44754</v>
       </c>
       <c r="G52" s="58">
-        <f>F52-E52</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H52" s="59">
@@ -13531,7 +13521,7 @@
         <v>44754</v>
       </c>
       <c r="J52" s="60">
-        <f>I52-H52</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K52" s="61">
@@ -13541,7 +13531,7 @@
     <row r="53" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="56"/>
       <c r="B53" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="C53" s="58" t="s">
@@ -13557,7 +13547,7 @@
         <v>44754</v>
       </c>
       <c r="G53" s="58">
-        <f>F53-E53</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H53" s="59">
@@ -13567,7 +13557,7 @@
         <v>44754</v>
       </c>
       <c r="J53" s="60">
-        <f>I53-H53</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K53" s="61">
@@ -13577,7 +13567,7 @@
     <row r="54" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="56"/>
       <c r="B54" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>46</v>
       </c>
       <c r="C54" s="58" t="s">
@@ -13593,7 +13583,7 @@
         <v>44754</v>
       </c>
       <c r="G54" s="58">
-        <f>F54-E54</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H54" s="59">
@@ -13603,7 +13593,7 @@
         <v>44754</v>
       </c>
       <c r="J54" s="60">
-        <f>I54-H54</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K54" s="61">
@@ -13613,7 +13603,7 @@
     <row r="55" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="56"/>
       <c r="B55" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>47</v>
       </c>
       <c r="C55" s="58" t="s">
@@ -13629,7 +13619,7 @@
         <v>44753</v>
       </c>
       <c r="G55" s="58">
-        <f>F55-E55</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H55" s="59">
@@ -13639,7 +13629,7 @@
         <v>44754</v>
       </c>
       <c r="J55" s="60">
-        <f>I55-H55</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K55" s="61">
@@ -13649,7 +13639,7 @@
     <row r="56" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="56"/>
       <c r="B56" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="C56" s="58" t="s">
@@ -13665,7 +13655,7 @@
         <v>44753</v>
       </c>
       <c r="G56" s="58">
-        <f>F56-E56</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H56" s="59">
@@ -13675,7 +13665,7 @@
         <v>44753</v>
       </c>
       <c r="J56" s="60">
-        <f>I56-H56</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K56" s="61">
@@ -13685,7 +13675,7 @@
     <row r="57" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="56"/>
       <c r="B57" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>49</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -13701,7 +13691,7 @@
         <v>44754</v>
       </c>
       <c r="G57" s="58">
-        <f>F57-E57</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H57" s="59">
@@ -13711,7 +13701,7 @@
         <v>44754</v>
       </c>
       <c r="J57" s="60">
-        <f>I57-H57</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K57" s="61">
@@ -13721,7 +13711,7 @@
     <row r="58" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="56"/>
       <c r="B58" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
       <c r="C58" s="58" t="s">
@@ -13737,7 +13727,7 @@
         <v>44754</v>
       </c>
       <c r="G58" s="58">
-        <f>F58-E58</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H58" s="59">
@@ -13747,7 +13737,7 @@
         <v>44754</v>
       </c>
       <c r="J58" s="60">
-        <f>I58-H58</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K58" s="61">
@@ -13757,7 +13747,7 @@
     <row r="59" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="56"/>
       <c r="B59" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>51</v>
       </c>
       <c r="C59" s="58" t="s">
@@ -13773,7 +13763,7 @@
         <v>44755</v>
       </c>
       <c r="G59" s="58">
-        <f>F59-E59</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H59" s="59">
@@ -13783,7 +13773,7 @@
         <v>44755</v>
       </c>
       <c r="J59" s="60">
-        <f>I59-H59</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K59" s="61">
@@ -13793,7 +13783,7 @@
     <row r="60" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="56"/>
       <c r="B60" s="112">
-        <f>ROW()-8</f>
+        <f t="shared" si="7"/>
         <v>52</v>
       </c>
       <c r="C60" s="58" t="s">
@@ -13809,7 +13799,7 @@
         <v>44753</v>
       </c>
       <c r="G60" s="58">
-        <f>F60-E60</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H60" s="59">
@@ -13819,7 +13809,7 @@
         <v>44753</v>
       </c>
       <c r="J60" s="60">
-        <f>I60-H60</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K60" s="61">
@@ -13842,7 +13832,7 @@
         <v>44753</v>
       </c>
       <c r="G61" s="58">
-        <f>F61-E61</f>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="H61" s="59">
@@ -13852,7 +13842,7 @@
         <v>44759</v>
       </c>
       <c r="J61" s="60">
-        <f>I61-H61</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="K61" s="61">
@@ -13875,18 +13865,18 @@
         <v>44770</v>
       </c>
       <c r="G62" s="58">
-        <f>F62-E62</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H62" s="59"/>
       <c r="I62" s="59"/>
       <c r="J62" s="60">
-        <f>I62-H62</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K62" s="107">
         <f>AVERAGE(K63:K115)</f>
-        <v>0.44622641509433941</v>
+        <v>0.4971698113207545</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="21" x14ac:dyDescent="0.25">
@@ -13907,13 +13897,13 @@
         <v>44770</v>
       </c>
       <c r="G63" s="58">
-        <f>F63-E63</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H63" s="59"/>
       <c r="I63" s="59"/>
       <c r="J63" s="60">
-        <f>I63-H63</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K63" s="61">
@@ -13941,13 +13931,13 @@
         <v>44770</v>
       </c>
       <c r="G64" s="58">
-        <f>F64-E64</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H64" s="59"/>
       <c r="I64" s="59"/>
       <c r="J64" s="60">
-        <f>I64-H64</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K64" s="61">
@@ -13975,7 +13965,7 @@
         <v>44770</v>
       </c>
       <c r="G65" s="58">
-        <f>F65-E65</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H65" s="59">
@@ -13985,7 +13975,7 @@
         <v>44761</v>
       </c>
       <c r="J65" s="60">
-        <f>I65-H65</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K65" s="61">
@@ -14013,7 +14003,7 @@
         <v>44770</v>
       </c>
       <c r="G66" s="58">
-        <f>F66-E66</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H66" s="59">
@@ -14023,7 +14013,7 @@
         <v>44761</v>
       </c>
       <c r="J66" s="60">
-        <f>I66-H66</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="K66" s="61">
@@ -14051,13 +14041,13 @@
         <v>44770</v>
       </c>
       <c r="G67" s="58">
-        <f>F67-E67</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H67" s="59"/>
       <c r="I67" s="59"/>
       <c r="J67" s="60">
-        <f>I67-H67</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K67" s="61">
@@ -14085,13 +14075,13 @@
         <v>44770</v>
       </c>
       <c r="G68" s="58">
-        <f>F68-E68</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H68" s="59"/>
       <c r="I68" s="59"/>
       <c r="J68" s="60">
-        <f>I68-H68</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K68" s="61">
@@ -14119,13 +14109,13 @@
         <v>44770</v>
       </c>
       <c r="G69" s="58">
-        <f>F69-E69</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H69" s="59"/>
       <c r="I69" s="106"/>
       <c r="J69" s="60">
-        <f>I69-H69</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K69" s="61">
@@ -14153,13 +14143,13 @@
         <v>44770</v>
       </c>
       <c r="G70" s="58">
-        <f>F70-E70</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H70" s="59"/>
       <c r="I70" s="59"/>
       <c r="J70" s="60">
-        <f>I70-H70</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K70" s="61">
@@ -14184,13 +14174,13 @@
         <v>44770</v>
       </c>
       <c r="G71" s="58">
-        <f>F71-E71</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H71" s="59"/>
       <c r="I71" s="59"/>
       <c r="J71" s="60">
-        <f>I71-H71</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K71" s="61">
@@ -14215,13 +14205,13 @@
         <v>44770</v>
       </c>
       <c r="G72" s="58">
-        <f>F72-E72</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H72" s="59"/>
       <c r="I72" s="59"/>
       <c r="J72" s="60">
-        <f>I72-H72</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K72" s="61">
@@ -14246,13 +14236,13 @@
         <v>44770</v>
       </c>
       <c r="G73" s="58">
-        <f>F73-E73</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H73" s="59"/>
       <c r="I73" s="59"/>
       <c r="J73" s="60">
-        <f>I73-H73</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K73" s="61">
@@ -14277,13 +14267,13 @@
         <v>44770</v>
       </c>
       <c r="G74" s="58">
-        <f>F74-E74</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H74" s="59"/>
       <c r="I74" s="59"/>
       <c r="J74" s="60">
-        <f>I74-H74</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K74" s="61">
@@ -14311,13 +14301,13 @@
         <v>44770</v>
       </c>
       <c r="G75" s="58">
-        <f>F75-E75</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H75" s="59"/>
       <c r="I75" s="105"/>
       <c r="J75" s="60">
-        <f>I75-H75</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K75" s="61">
@@ -14345,13 +14335,13 @@
         <v>44770</v>
       </c>
       <c r="G76" s="58">
-        <f>F76-E76</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H76" s="59"/>
       <c r="I76" s="59"/>
       <c r="J76" s="60">
-        <f>I76-H76</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K76" s="61">
@@ -14376,13 +14366,13 @@
         <v>44770</v>
       </c>
       <c r="G77" s="58">
-        <f>F77-E77</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H77" s="59"/>
       <c r="I77" s="59"/>
       <c r="J77" s="60">
-        <f>I77-H77</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K77" s="61">
@@ -14410,13 +14400,13 @@
         <v>44770</v>
       </c>
       <c r="G78" s="58">
-        <f>F78-E78</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H78" s="59"/>
       <c r="I78" s="59"/>
       <c r="J78" s="60">
-        <f>I78-H78</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K78" s="61">
@@ -14444,13 +14434,13 @@
         <v>44770</v>
       </c>
       <c r="G79" s="58">
-        <f>F79-E79</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="H79" s="59"/>
       <c r="I79" s="59"/>
       <c r="J79" s="60">
-        <f>I79-H79</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="K79" s="61">
@@ -14478,13 +14468,13 @@
         <v>44770</v>
       </c>
       <c r="G80" s="58">
-        <f>F80-E80</f>
+        <f t="shared" ref="G80:G111" si="12">F80-E80</f>
         <v>13</v>
       </c>
       <c r="H80" s="59"/>
       <c r="I80" s="59"/>
       <c r="J80" s="60">
-        <f>I80-H80</f>
+        <f t="shared" ref="J80:J111" si="13">I80-H80</f>
         <v>0</v>
       </c>
       <c r="K80" s="61">
@@ -14496,32 +14486,32 @@
     </row>
     <row r="81" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A81" s="56"/>
-      <c r="B81" s="171">
+      <c r="B81" s="129">
         <v>19</v>
       </c>
-      <c r="C81" s="172" t="s">
+      <c r="C81" s="130" t="s">
         <v>119</v>
       </c>
-      <c r="D81" s="173" t="s">
+      <c r="D81" s="131" t="s">
         <v>132</v>
       </c>
-      <c r="E81" s="174">
+      <c r="E81" s="132">
         <v>44757</v>
       </c>
-      <c r="F81" s="174">
+      <c r="F81" s="132">
         <v>44770</v>
       </c>
-      <c r="G81" s="172">
-        <f>F81-E81</f>
+      <c r="G81" s="130">
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
-      <c r="H81" s="174"/>
-      <c r="I81" s="174"/>
-      <c r="J81" s="175">
-        <f>I81-H81</f>
+      <c r="H81" s="132"/>
+      <c r="I81" s="132"/>
+      <c r="J81" s="133">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="K81" s="176">
+      <c r="K81" s="134">
         <v>0.5</v>
       </c>
       <c r="L81" t="s">
@@ -14546,13 +14536,13 @@
         <v>44770</v>
       </c>
       <c r="G82" s="58">
-        <f>F82-E82</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H82" s="59"/>
       <c r="I82" s="59"/>
       <c r="J82" s="60">
-        <f>I82-H82</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K82" s="61">
@@ -14580,13 +14570,13 @@
         <v>44770</v>
       </c>
       <c r="G83" s="58">
-        <f>F83-E83</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H83" s="59"/>
       <c r="I83" s="59"/>
       <c r="J83" s="60">
-        <f>I83-H83</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K83" s="61">
@@ -14614,13 +14604,13 @@
         <v>44770</v>
       </c>
       <c r="G84" s="58">
-        <f>F84-E84</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H84" s="59"/>
       <c r="I84" s="59"/>
       <c r="J84" s="60">
-        <f>I84-H84</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K84" s="61">
@@ -14648,13 +14638,13 @@
         <v>44770</v>
       </c>
       <c r="G85" s="58">
-        <f>F85-E85</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H85" s="59"/>
       <c r="I85" s="59"/>
       <c r="J85" s="60">
-        <f>I85-H85</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K85" s="61">
@@ -14682,13 +14672,13 @@
         <v>44770</v>
       </c>
       <c r="G86" s="58">
-        <f>F86-E86</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H86" s="59"/>
       <c r="I86" s="59"/>
       <c r="J86" s="60">
-        <f>I86-H86</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K86" s="61">
@@ -14716,17 +14706,21 @@
         <v>44770</v>
       </c>
       <c r="G87" s="58">
-        <f>F87-E87</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
-      <c r="H87" s="59"/>
-      <c r="I87" s="59"/>
+      <c r="H87" s="59">
+        <v>44760</v>
+      </c>
+      <c r="I87" s="59">
+        <v>44761</v>
+      </c>
       <c r="J87" s="60">
-        <f>I87-H87</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="K87" s="61">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="L87">
         <v>1</v>
@@ -14750,13 +14744,13 @@
         <v>44770</v>
       </c>
       <c r="G88" s="58">
-        <f>F88-E88</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H88" s="59"/>
       <c r="I88" s="59"/>
       <c r="J88" s="60">
-        <f>I88-H88</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K88" s="61">
@@ -14784,13 +14778,13 @@
         <v>44770</v>
       </c>
       <c r="G89" s="58">
-        <f>F89-E89</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H89" s="59"/>
       <c r="I89" s="59"/>
       <c r="J89" s="60">
-        <f>I89-H89</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K89" s="61">
@@ -14818,17 +14812,17 @@
         <v>44770</v>
       </c>
       <c r="G90" s="58">
-        <f>F90-E90</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H90" s="59"/>
       <c r="I90" s="59"/>
       <c r="J90" s="60">
-        <f>I90-H90</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K90" s="61">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="L90">
         <v>2</v>
@@ -14852,17 +14846,17 @@
         <v>44770</v>
       </c>
       <c r="G91" s="58">
-        <f>F91-E91</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H91" s="59"/>
       <c r="I91" s="59"/>
       <c r="J91" s="60">
-        <f>I91-H91</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K91" s="61">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="L91">
         <v>0</v>
@@ -14886,13 +14880,13 @@
         <v>44770</v>
       </c>
       <c r="G92" s="58">
-        <f>F92-E92</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H92" s="59"/>
       <c r="I92" s="59"/>
       <c r="J92" s="60">
-        <f>I92-H92</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K92" s="61">
@@ -14917,13 +14911,13 @@
         <v>44770</v>
       </c>
       <c r="G93" s="58">
-        <f>F93-E93</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H93" s="59"/>
       <c r="I93" s="59"/>
       <c r="J93" s="60">
-        <f>I93-H93</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K93" s="61">
@@ -14948,13 +14942,13 @@
         <v>44770</v>
       </c>
       <c r="G94" s="58">
-        <f>F94-E94</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H94" s="59"/>
       <c r="I94" s="59"/>
       <c r="J94" s="60">
-        <f>I94-H94</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K94" s="61">
@@ -14979,13 +14973,13 @@
         <v>44770</v>
       </c>
       <c r="G95" s="58">
-        <f>F95-E95</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H95" s="59"/>
       <c r="I95" s="59"/>
       <c r="J95" s="60">
-        <f>I95-H95</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K95" s="61">
@@ -15013,13 +15007,13 @@
         <v>44770</v>
       </c>
       <c r="G96" s="58">
-        <f>F96-E96</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H96" s="59"/>
       <c r="I96" s="59"/>
       <c r="J96" s="60">
-        <f>I96-H96</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K96" s="61">
@@ -15047,13 +15041,13 @@
         <v>44770</v>
       </c>
       <c r="G97" s="58">
-        <f>F97-E97</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H97" s="59"/>
       <c r="I97" s="59"/>
       <c r="J97" s="60">
-        <f>I97-H97</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K97" s="61">
@@ -15081,13 +15075,13 @@
         <v>44770</v>
       </c>
       <c r="G98" s="58">
-        <f>F98-E98</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H98" s="59"/>
       <c r="I98" s="59"/>
       <c r="J98" s="60">
-        <f>I98-H98</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K98" s="61">
@@ -15115,17 +15109,21 @@
         <v>44770</v>
       </c>
       <c r="G99" s="58">
-        <f>F99-E99</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
-      <c r="H99" s="59"/>
-      <c r="I99" s="59"/>
+      <c r="H99" s="59">
+        <v>44760</v>
+      </c>
+      <c r="I99" s="59">
+        <v>44761</v>
+      </c>
       <c r="J99" s="60">
-        <f>I99-H99</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="K99" s="61">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L99">
         <v>1</v>
@@ -15149,13 +15147,13 @@
         <v>44770</v>
       </c>
       <c r="G100" s="58">
-        <f>F100-E100</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H100" s="59"/>
       <c r="I100" s="105"/>
       <c r="J100" s="60">
-        <f>I100-H100</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K100" s="61">
@@ -15183,13 +15181,13 @@
         <v>44770</v>
       </c>
       <c r="G101" s="124">
-        <f>F101-E101</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H101" s="125"/>
       <c r="I101" s="126"/>
       <c r="J101" s="127">
-        <f>I101-H101</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K101" s="128">
@@ -15217,13 +15215,13 @@
         <v>44770</v>
       </c>
       <c r="G102" s="58">
-        <f>F102-E102</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H102" s="59"/>
       <c r="I102" s="59"/>
       <c r="J102" s="60">
-        <f>I102-H102</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K102" s="61">
@@ -15248,13 +15246,13 @@
         <v>44770</v>
       </c>
       <c r="G103" s="58">
-        <f>F103-E103</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H103" s="59"/>
       <c r="I103" s="59"/>
       <c r="J103" s="60">
-        <f>I103-H103</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K103" s="61">
@@ -15279,13 +15277,13 @@
         <v>44770</v>
       </c>
       <c r="G104" s="58">
-        <f>F104-E104</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H104" s="59"/>
       <c r="I104" s="59"/>
       <c r="J104" s="60">
-        <f>I104-H104</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K104" s="61">
@@ -15313,13 +15311,13 @@
         <v>44770</v>
       </c>
       <c r="G105" s="58">
-        <f>F105-E105</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H105" s="59"/>
       <c r="I105" s="59"/>
       <c r="J105" s="60">
-        <f>I105-H105</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K105" s="61">
@@ -15347,13 +15345,13 @@
         <v>44770</v>
       </c>
       <c r="G106" s="58">
-        <f>F106-E106</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H106" s="59"/>
       <c r="I106" s="59"/>
       <c r="J106" s="60">
-        <f>I106-H106</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K106" s="61">
@@ -15381,13 +15379,13 @@
         <v>44770</v>
       </c>
       <c r="G107" s="58">
-        <f>F107-E107</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H107" s="59"/>
       <c r="I107" s="59"/>
       <c r="J107" s="60">
-        <f>I107-H107</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K107" s="61">
@@ -15415,13 +15413,13 @@
         <v>44770</v>
       </c>
       <c r="G108" s="58">
-        <f>F108-E108</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H108" s="59"/>
       <c r="I108" s="59"/>
       <c r="J108" s="60">
-        <f>I108-H108</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K108" s="61">
@@ -15449,13 +15447,13 @@
         <v>44770</v>
       </c>
       <c r="G109" s="58">
-        <f>F109-E109</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H109" s="59"/>
       <c r="I109" s="59"/>
       <c r="J109" s="60">
-        <f>I109-H109</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K109" s="61">
@@ -15483,13 +15481,13 @@
         <v>44770</v>
       </c>
       <c r="G110" s="58">
-        <f>F110-E110</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H110" s="59"/>
       <c r="I110" s="59"/>
       <c r="J110" s="60">
-        <f>I110-H110</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K110" s="61">
@@ -15517,13 +15515,13 @@
         <v>44770</v>
       </c>
       <c r="G111" s="58">
-        <f>F111-E111</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H111" s="59"/>
       <c r="I111" s="59"/>
       <c r="J111" s="60">
-        <f>I111-H111</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="K111" s="61">
@@ -15551,13 +15549,13 @@
         <v>44770</v>
       </c>
       <c r="G112" s="58">
-        <f>F112-E112</f>
+        <f t="shared" ref="G112:G143" si="14">F112-E112</f>
         <v>13</v>
       </c>
       <c r="H112" s="59"/>
       <c r="I112" s="59"/>
       <c r="J112" s="60">
-        <f>I112-H112</f>
+        <f t="shared" ref="J112:J143" si="15">I112-H112</f>
         <v>0</v>
       </c>
       <c r="K112" s="61">
@@ -15585,13 +15583,13 @@
         <v>44770</v>
       </c>
       <c r="G113" s="58">
-        <f>F113-E113</f>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="H113" s="59"/>
       <c r="I113" s="59"/>
       <c r="J113" s="60">
-        <f>I113-H113</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="K113" s="61">
@@ -15619,13 +15617,13 @@
         <v>44770</v>
       </c>
       <c r="G114" s="58">
-        <f>F114-E114</f>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="H114" s="59"/>
       <c r="I114" s="59"/>
       <c r="J114" s="60">
-        <f>I114-H114</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="K114" s="61">
@@ -15647,7 +15645,7 @@
       <c r="E115" s="59"/>
       <c r="F115" s="59"/>
       <c r="G115" s="58">
-        <f t="shared" ref="G115:G116" si="7">F115-E115</f>
+        <f t="shared" ref="G115:G116" si="16">F115-E115</f>
         <v>0</v>
       </c>
       <c r="H115" s="59"/>
@@ -15672,7 +15670,7 @@
       <c r="E116" s="59"/>
       <c r="F116" s="59"/>
       <c r="G116" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H116" s="59"/>
@@ -15820,51 +15818,51 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="141" t="str">
+      <c r="B2" s="144"/>
+      <c r="C2" s="147" t="str">
         <f>Cover!E40</f>
         <v xml:space="preserve">Level Up </v>
       </c>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="142"/>
-      <c r="L2" s="142"/>
-      <c r="M2" s="142"/>
-      <c r="N2" s="142"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
+      <c r="L2" s="148"/>
+      <c r="M2" s="148"/>
+      <c r="N2" s="148"/>
       <c r="O2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="145"/>
-      <c r="Q2" s="146"/>
+      <c r="P2" s="151"/>
+      <c r="Q2" s="152"/>
     </row>
     <row r="3" spans="1:17" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="139"/>
-      <c r="B3" s="140"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="144"/>
+      <c r="A3" s="145"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="150"/>
+      <c r="K3" s="150"/>
+      <c r="L3" s="150"/>
+      <c r="M3" s="150"/>
+      <c r="N3" s="150"/>
       <c r="O3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="147"/>
-      <c r="Q3" s="148"/>
+      <c r="P3" s="153"/>
+      <c r="Q3" s="154"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
@@ -15874,89 +15872,89 @@
       <c r="A5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="155"/>
-      <c r="E5" s="156"/>
-      <c r="F5" s="156"/>
-      <c r="G5" s="156"/>
-      <c r="H5" s="156"/>
-      <c r="I5" s="156"/>
-      <c r="J5" s="156"/>
-      <c r="K5" s="156"/>
-      <c r="L5" s="156"/>
-      <c r="M5" s="156"/>
-      <c r="N5" s="156"/>
-      <c r="O5" s="156"/>
-      <c r="P5" s="157"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="162"/>
+      <c r="H5" s="162"/>
+      <c r="I5" s="162"/>
+      <c r="J5" s="162"/>
+      <c r="K5" s="162"/>
+      <c r="L5" s="162"/>
+      <c r="M5" s="162"/>
+      <c r="N5" s="162"/>
+      <c r="O5" s="162"/>
+      <c r="P5" s="163"/>
       <c r="Q5" s="13"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="158"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
-      <c r="J6" s="159"/>
-      <c r="K6" s="159"/>
-      <c r="L6" s="159"/>
-      <c r="M6" s="159"/>
-      <c r="N6" s="159"/>
-      <c r="O6" s="159"/>
-      <c r="P6" s="160"/>
+      <c r="D6" s="164"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
+      <c r="J6" s="165"/>
+      <c r="K6" s="165"/>
+      <c r="L6" s="165"/>
+      <c r="M6" s="165"/>
+      <c r="N6" s="165"/>
+      <c r="O6" s="165"/>
+      <c r="P6" s="166"/>
       <c r="Q6" s="13"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="159"/>
-      <c r="F7" s="159"/>
-      <c r="G7" s="159"/>
-      <c r="H7" s="159"/>
-      <c r="I7" s="159"/>
-      <c r="J7" s="159"/>
-      <c r="K7" s="159"/>
-      <c r="L7" s="159"/>
-      <c r="M7" s="159"/>
-      <c r="N7" s="159"/>
-      <c r="O7" s="159"/>
-      <c r="P7" s="160"/>
+      <c r="D7" s="164"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="165"/>
+      <c r="H7" s="165"/>
+      <c r="I7" s="165"/>
+      <c r="J7" s="165"/>
+      <c r="K7" s="165"/>
+      <c r="L7" s="165"/>
+      <c r="M7" s="165"/>
+      <c r="N7" s="165"/>
+      <c r="O7" s="165"/>
+      <c r="P7" s="166"/>
       <c r="Q7" s="13"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
-      <c r="D8" s="158"/>
-      <c r="E8" s="159"/>
-      <c r="F8" s="159"/>
-      <c r="G8" s="159"/>
-      <c r="H8" s="159"/>
-      <c r="I8" s="159"/>
-      <c r="J8" s="159"/>
-      <c r="K8" s="159"/>
-      <c r="L8" s="159"/>
-      <c r="M8" s="159"/>
-      <c r="N8" s="159"/>
-      <c r="O8" s="159"/>
-      <c r="P8" s="160"/>
+      <c r="D8" s="164"/>
+      <c r="E8" s="165"/>
+      <c r="F8" s="165"/>
+      <c r="G8" s="165"/>
+      <c r="H8" s="165"/>
+      <c r="I8" s="165"/>
+      <c r="J8" s="165"/>
+      <c r="K8" s="165"/>
+      <c r="L8" s="165"/>
+      <c r="M8" s="165"/>
+      <c r="N8" s="165"/>
+      <c r="O8" s="165"/>
+      <c r="P8" s="166"/>
       <c r="Q8" s="13"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
-      <c r="D9" s="161"/>
-      <c r="E9" s="162"/>
-      <c r="F9" s="162"/>
-      <c r="G9" s="162"/>
-      <c r="H9" s="162"/>
-      <c r="I9" s="162"/>
-      <c r="J9" s="162"/>
-      <c r="K9" s="162"/>
-      <c r="L9" s="162"/>
-      <c r="M9" s="162"/>
-      <c r="N9" s="162"/>
-      <c r="O9" s="162"/>
-      <c r="P9" s="163"/>
+      <c r="D9" s="167"/>
+      <c r="E9" s="168"/>
+      <c r="F9" s="168"/>
+      <c r="G9" s="168"/>
+      <c r="H9" s="168"/>
+      <c r="I9" s="168"/>
+      <c r="J9" s="168"/>
+      <c r="K9" s="168"/>
+      <c r="L9" s="168"/>
+      <c r="M9" s="168"/>
+      <c r="N9" s="168"/>
+      <c r="O9" s="168"/>
+      <c r="P9" s="169"/>
       <c r="Q9" s="13"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -15964,44 +15962,44 @@
       <c r="Q10" s="13"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="149" t="s">
+      <c r="A11" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="150"/>
-      <c r="C11" s="150"/>
-      <c r="D11" s="150"/>
-      <c r="E11" s="150"/>
-      <c r="F11" s="150"/>
-      <c r="G11" s="150"/>
-      <c r="H11" s="150"/>
-      <c r="I11" s="150"/>
-      <c r="J11" s="150"/>
-      <c r="K11" s="150"/>
-      <c r="L11" s="150"/>
-      <c r="M11" s="150"/>
-      <c r="N11" s="150"/>
-      <c r="O11" s="150"/>
-      <c r="P11" s="150"/>
-      <c r="Q11" s="151"/>
+      <c r="B11" s="156"/>
+      <c r="C11" s="156"/>
+      <c r="D11" s="156"/>
+      <c r="E11" s="156"/>
+      <c r="F11" s="156"/>
+      <c r="G11" s="156"/>
+      <c r="H11" s="156"/>
+      <c r="I11" s="156"/>
+      <c r="J11" s="156"/>
+      <c r="K11" s="156"/>
+      <c r="L11" s="156"/>
+      <c r="M11" s="156"/>
+      <c r="N11" s="156"/>
+      <c r="O11" s="156"/>
+      <c r="P11" s="156"/>
+      <c r="Q11" s="157"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="152"/>
-      <c r="B12" s="153"/>
-      <c r="C12" s="153"/>
-      <c r="D12" s="153"/>
-      <c r="E12" s="153"/>
-      <c r="F12" s="153"/>
-      <c r="G12" s="153"/>
-      <c r="H12" s="153"/>
-      <c r="I12" s="153"/>
-      <c r="J12" s="153"/>
-      <c r="K12" s="153"/>
-      <c r="L12" s="153"/>
-      <c r="M12" s="153"/>
-      <c r="N12" s="153"/>
-      <c r="O12" s="153"/>
-      <c r="P12" s="153"/>
-      <c r="Q12" s="154"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="159"/>
+      <c r="C12" s="159"/>
+      <c r="D12" s="159"/>
+      <c r="E12" s="159"/>
+      <c r="F12" s="159"/>
+      <c r="G12" s="159"/>
+      <c r="H12" s="159"/>
+      <c r="I12" s="159"/>
+      <c r="J12" s="159"/>
+      <c r="K12" s="159"/>
+      <c r="L12" s="159"/>
+      <c r="M12" s="159"/>
+      <c r="N12" s="159"/>
+      <c r="O12" s="159"/>
+      <c r="P12" s="159"/>
+      <c r="Q12" s="160"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
@@ -16406,51 +16404,51 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="141" t="str">
+      <c r="B2" s="144"/>
+      <c r="C2" s="147" t="str">
         <f>Cover!E40</f>
         <v xml:space="preserve">Level Up </v>
       </c>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="142"/>
-      <c r="L2" s="142"/>
-      <c r="M2" s="142"/>
-      <c r="N2" s="142"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
+      <c r="L2" s="148"/>
+      <c r="M2" s="148"/>
+      <c r="N2" s="148"/>
       <c r="O2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="145"/>
-      <c r="Q2" s="146"/>
+      <c r="P2" s="151"/>
+      <c r="Q2" s="152"/>
     </row>
     <row r="3" spans="1:17" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="139"/>
-      <c r="B3" s="140"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="144"/>
+      <c r="A3" s="145"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="150"/>
+      <c r="K3" s="150"/>
+      <c r="L3" s="150"/>
+      <c r="M3" s="150"/>
+      <c r="N3" s="150"/>
       <c r="O3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="147"/>
-      <c r="Q3" s="148"/>
+      <c r="P3" s="153"/>
+      <c r="Q3" s="154"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
@@ -16777,56 +16775,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="170" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="141" t="str">
+      <c r="B1" s="171"/>
+      <c r="C1" s="147" t="str">
         <f>[1]Cover!A31</f>
         <v>Food_Lab</v>
       </c>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
-      <c r="K1" s="142"/>
-      <c r="L1" s="142"/>
-      <c r="M1" s="142"/>
-      <c r="N1" s="142"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
+      <c r="H1" s="148"/>
+      <c r="I1" s="148"/>
+      <c r="J1" s="148"/>
+      <c r="K1" s="148"/>
+      <c r="L1" s="148"/>
+      <c r="M1" s="148"/>
+      <c r="N1" s="148"/>
       <c r="O1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="145">
+      <c r="P1" s="151">
         <v>44555</v>
       </c>
-      <c r="Q1" s="146"/>
+      <c r="Q1" s="152"/>
     </row>
     <row r="2" spans="1:19" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="166"/>
-      <c r="B2" s="167"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
-      <c r="I2" s="144"/>
-      <c r="J2" s="144"/>
-      <c r="K2" s="144"/>
-      <c r="L2" s="144"/>
-      <c r="M2" s="144"/>
-      <c r="N2" s="144"/>
+      <c r="A2" s="172"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
+      <c r="J2" s="150"/>
+      <c r="K2" s="150"/>
+      <c r="L2" s="150"/>
+      <c r="M2" s="150"/>
+      <c r="N2" s="150"/>
       <c r="O2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="147">
+      <c r="P2" s="153">
         <f ca="1">NOW()</f>
-        <v>44766.857009259256</v>
-      </c>
-      <c r="Q2" s="148"/>
+        <v>44769.489709606481</v>
+      </c>
+      <c r="Q2" s="154"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
@@ -18255,47 +18253,47 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="141" t="str">
+      <c r="B2" s="144"/>
+      <c r="C2" s="147" t="str">
         <f>Cover!E40</f>
         <v xml:space="preserve">Level Up </v>
       </c>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="142"/>
-      <c r="L2" s="142"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="148"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="148"/>
+      <c r="L2" s="148"/>
       <c r="M2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="145"/>
-      <c r="O2" s="146"/>
+      <c r="N2" s="151"/>
+      <c r="O2" s="152"/>
     </row>
     <row r="3" spans="1:15" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="139"/>
-      <c r="B3" s="140"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
+      <c r="A3" s="145"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="150"/>
+      <c r="K3" s="150"/>
+      <c r="L3" s="150"/>
       <c r="M3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="147"/>
-      <c r="O3" s="148"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="154"/>
     </row>
     <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
@@ -18737,19 +18735,19 @@
     </row>
     <row r="3" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D3" s="78"/>
-      <c r="E3" s="169">
+      <c r="E3" s="175">
         <v>1</v>
       </c>
       <c r="F3" s="79" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="169">
+      <c r="G3" s="175">
         <v>2</v>
       </c>
       <c r="H3" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="169">
+      <c r="I3" s="175">
         <v>3</v>
       </c>
       <c r="J3" s="81" t="s">
@@ -18759,15 +18757,15 @@
     </row>
     <row r="4" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D4" s="78"/>
-      <c r="E4" s="169"/>
+      <c r="E4" s="175"/>
       <c r="F4" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="169"/>
+      <c r="G4" s="175"/>
       <c r="H4" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="169"/>
+      <c r="I4" s="175"/>
       <c r="J4" s="74" t="s">
         <v>51</v>
       </c>
@@ -18778,15 +18776,15 @@
     </row>
     <row r="5" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D5" s="78"/>
-      <c r="E5" s="169"/>
+      <c r="E5" s="175"/>
       <c r="F5" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="169"/>
+      <c r="G5" s="175"/>
       <c r="H5" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="I5" s="169"/>
+      <c r="I5" s="175"/>
       <c r="J5" s="74" t="s">
         <v>50</v>
       </c>
@@ -18820,13 +18818,13 @@
     </row>
     <row r="8" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D8" s="78"/>
-      <c r="E8" s="169">
+      <c r="E8" s="175">
         <v>4</v>
       </c>
       <c r="F8" s="86" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="169">
+      <c r="G8" s="175">
         <v>5</v>
       </c>
       <c r="H8" s="87" t="s">
@@ -18836,11 +18834,11 @@
     </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D9" s="78"/>
-      <c r="E9" s="169"/>
+      <c r="E9" s="175"/>
       <c r="F9" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="169"/>
+      <c r="G9" s="175"/>
       <c r="H9" s="74" t="s">
         <v>75</v>
       </c>
@@ -18848,9 +18846,9 @@
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D10" s="83"/>
-      <c r="E10" s="170"/>
+      <c r="E10" s="176"/>
       <c r="F10" s="84"/>
-      <c r="G10" s="170"/>
+      <c r="G10" s="176"/>
       <c r="H10" s="84"/>
       <c r="I10" s="84"/>
       <c r="J10" s="84"/>
@@ -18874,14 +18872,14 @@
     </row>
     <row r="12" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D12" s="78"/>
-      <c r="F12" s="168" t="s">
+      <c r="F12" s="174" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="168"/>
-      <c r="H12" s="168"/>
-      <c r="I12" s="168"/>
-      <c r="J12" s="168"/>
-      <c r="K12" s="168"/>
+      <c r="G12" s="174"/>
+      <c r="H12" s="174"/>
+      <c r="I12" s="174"/>
+      <c r="J12" s="174"/>
+      <c r="K12" s="174"/>
       <c r="N12" s="82"/>
     </row>
     <row r="13" spans="4:14" x14ac:dyDescent="0.3">

</xml_diff>